<commit_message>
Now the script can add 1 or more recipes
</commit_message>
<xml_diff>
--- a/Recipes_Database.xlsx
+++ b/Recipes_Database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Control_sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
   <si>
     <t xml:space="preserve">Recipe Name</t>
   </si>
@@ -164,10 +164,10 @@
     <t xml:space="preserve">Black Pepper</t>
   </si>
   <si>
-    <t xml:space="preserve">Wholewheat pasta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shallot</t>
+    <t xml:space="preserve">Wholewheat Pasta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shallot</t>
   </si>
   <si>
     <t xml:space="preserve">Frozen peas</t>
@@ -189,12 +189,6 @@
   </si>
   <si>
     <t xml:space="preserve">Vegetable stock cube</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chives</t>
   </si>
 </sst>
 </file>
@@ -305,9 +299,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>21600</xdr:colOff>
+      <xdr:colOff>21240</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -320,8 +314,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4438440" y="169560"/>
-          <a:ext cx="3271680" cy="3567240"/>
+          <a:off x="4443840" y="169560"/>
+          <a:ext cx="3276000" cy="3566880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -343,11 +337,11 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.88"/>
@@ -378,6 +372,9 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -407,7 +404,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.67"/>
   </cols>
@@ -536,7 +533,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -619,7 +616,7 @@
       <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.52"/>
@@ -804,13 +801,13 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.88"/>
   </cols>
@@ -907,7 +904,7 @@
         <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>1</v>
@@ -918,7 +915,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Script can add one or more recipes
</commit_message>
<xml_diff>
--- a/Recipes_Database.xlsx
+++ b/Recipes_Database.xlsx
@@ -5,14 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Control_sheet" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Pesto_Pasta" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Chicken_Jambaella" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Mushroom_risotto" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Salmon_Pasta" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="House_Stock" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Pesto_Pasta" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Chicken_Jambaella" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Mushroom_risotto" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Salmon_Pasta" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="57">
   <si>
     <t xml:space="preserve">Recipe Name</t>
   </si>
@@ -32,12 +33,15 @@
     <t xml:space="preserve">Selected?</t>
   </si>
   <si>
+    <t xml:space="preserve">House_Stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pesto_Pasta</t>
   </si>
   <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
     <t xml:space="preserve">Beef_Stirfry</t>
   </si>
   <si>
@@ -62,6 +66,21 @@
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
+    <t xml:space="preserve">Red Onion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">piece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmon Fillets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fish</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pesto</t>
   </si>
   <si>
@@ -89,9 +108,6 @@
     <t xml:space="preserve">Red Pepper</t>
   </si>
   <si>
-    <t xml:space="preserve">Veg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Onion</t>
   </si>
   <si>
@@ -149,9 +165,6 @@
     <t xml:space="preserve">Herbs</t>
   </si>
   <si>
-    <t xml:space="preserve">piece</t>
-  </si>
-  <si>
     <t xml:space="preserve">Parmesan Cheese</t>
   </si>
   <si>
@@ -174,12 +187,6 @@
   </si>
   <si>
     <t xml:space="preserve">Freezer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salmon fillets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fish</t>
   </si>
   <si>
     <t xml:space="preserve">Low-Fat crème fraiche</t>
@@ -263,13 +270,9 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -299,9 +302,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>21240</xdr:colOff>
+      <xdr:colOff>20880</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -314,8 +317,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4443840" y="169560"/>
-          <a:ext cx="3276000" cy="3566880"/>
+          <a:off x="4448880" y="169560"/>
+          <a:ext cx="3280680" cy="3566520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -335,13 +338,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.88"/>
@@ -368,18 +371,26 @@
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -398,116 +409,188 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.42"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>250</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -522,7 +605,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -533,254 +616,65 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>250</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.88"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>500</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>500</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>340</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>125</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -799,13 +693,202 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.88"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>340</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.52"/>
@@ -813,118 +896,118 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D1" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>140</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>